<commit_message>
gráficos gestión y fomento
</commit_message>
<xml_diff>
--- a/Fuentes/Bienestar.xlsx
+++ b/Fuentes/Bienestar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UNIVERSIDAD NACIONAL\Documents\Sistema Estadistico\Repositorios de GitHub\Plan Global\PGD\Fuentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A81B29-0BDD-4BA4-8F97-6AC36DE713A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE11C736-C61C-4C27-8136-E0A8C67EC96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="698" xr2:uid="{BCF827EF-10EC-4D49-AFB0-F3B46FDF3606}"/>
   </bookViews>
@@ -149,9 +149,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Periodo</t>
-  </si>
-  <si>
     <t>Programa</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Usos</t>
+  </si>
+  <si>
+    <t>Periodof</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -565,16 +565,16 @@
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1539,7 +1539,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1556,16 +1556,16 @@
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2531,7 +2531,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2548,16 +2548,16 @@
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3284,7 +3284,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -3297,16 +3297,16 @@
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4271,7 +4271,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -4285,13 +4285,13 @@
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>